<commit_message>
Fixed failed scripts in Dralogin
</commit_message>
<xml_diff>
--- a/src/test/test-data/SsoLoginTestData.xlsx
+++ b/src/test/test-data/SsoLoginTestData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\API Project\1p-api-automation\src\test\test-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -74,9 +69,6 @@
     <t>?entityId=http://abc.com&amp;app=dra</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>?entityId=http://ec2-35-162-11-166.us-west-2.compute.amazonaws.com:8080/auth/realms/Platform-IAM&amp;app=dra</t>
   </si>
   <si>
@@ -128,9 +120,6 @@
     <t>status=200||code=90071||message=Identity provider does not have a ShibOrg set up for Neon</t>
   </si>
   <si>
-    <t>status=200||lastName=nottiedtosubscription||email=test.user101@clarivate.com</t>
-  </si>
-  <si>
     <t>OPQA-5695</t>
   </si>
   <si>
@@ -243,9 +232,6 @@
   </si>
   <si>
     <t>status=200||code=90072</t>
-  </si>
-  <si>
-    <t>status=200||firstName=userexists||email=test.user101@clarivate.com</t>
   </si>
   <si>
     <t>OPQA-5713</t>
@@ -325,9 +311,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,7 +405,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -443,9 +428,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,7 +489,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,10 +521,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,7 +555,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -750,28 +730,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="85.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="62.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="57.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="85.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="62.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="57.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,12 +789,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -827,7 +807,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -835,16 +815,14 @@
         <v>15</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -862,32 +840,30 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -895,605 +871,561 @@
         <v>15</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K5" s="2"/>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K6" s="2"/>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" ht="30.75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" ht="23.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="75">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="29.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10"/>
+        <v>91</v>
+      </c>
       <c r="H10" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="2"/>
-      <c r="L10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" ht="29.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" ht="29.25" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="29.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="29.25" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" ht="32.25" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="43.5" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="44.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="48.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="33.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="48" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="18.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="L21" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J16" r:id="rId1"/>
-    <hyperlink ref="J12" r:id="rId2"/>
+    <hyperlink ref="J16" r:id="rId1" display="status=200||lastName=nottiedtosubscription||email=test.user101@clarivate.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed failed script in SSologin module
</commit_message>
<xml_diff>
--- a/src/test/test-data/SsoLoginTestData.xlsx
+++ b/src/test/test-data/SsoLoginTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -306,6 +306,9 @@
   <si>
     <t>{"RelayState":"(OPQA-5697_relayState)",
 "SAMLResponse":"InvalidSAML"}</t>
+  </si>
+  <si>
+    <t>status=200||lastName=nottiedtosubscription</t>
   </si>
 </sst>
 </file>
@@ -733,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L25"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1233,7 +1236,7 @@
         <v>40</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>

</xml_diff>

<commit_message>
Modified validations in ssologin module
</commit_message>
<xml_diff>
--- a/src/test/test-data/SsoLoginTestData.xlsx
+++ b/src/test/test-data/SsoLoginTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -306,6 +306,9 @@
   <si>
     <t>{"RelayState":"(OPQA-5697_relayState)",
 "SAMLResponse":"InvalidSAML"}</t>
+  </si>
+  <si>
+    <t>status=200||lastName=nottiedtosubscription||email=test.user101@clarivate.com</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -428,6 +431,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -733,8 +739,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+      <pane ySplit="900" topLeftCell="A10" activePane="bottomLeft"/>
+      <selection activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -815,7 +823,6 @@
         <v>15</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="2" t="s">
@@ -843,7 +850,6 @@
         <v>18</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="2" t="s">
@@ -873,7 +879,6 @@
       <c r="K4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="2" t="s">
@@ -959,7 +964,6 @@
       <c r="K7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="23.25" customHeight="1">
       <c r="A8" s="5" t="s">
@@ -989,7 +993,6 @@
         <v>29</v>
       </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="75">
       <c r="A9" s="5" t="s">
@@ -1019,7 +1022,6 @@
         <v>31</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="29.25" customHeight="1">
       <c r="A10" s="2" t="s">
@@ -1112,7 +1114,6 @@
         <v>15</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="29.25" customHeight="1">
       <c r="A13" s="2" t="s">
@@ -1204,7 +1205,6 @@
         <v>33</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="43.5" customHeight="1">
       <c r="A16" s="2" t="s">
@@ -1232,13 +1232,12 @@
       <c r="I16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>67</v>
+      <c r="J16" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="44.25" customHeight="1">
+    </row>
+    <row r="17" spans="1:11" ht="44.25" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -1268,9 +1267,8 @@
         <v>67</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" ht="48.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:11" ht="48.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>59</v>
       </c>
@@ -1300,9 +1298,8 @@
         <v>70</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" ht="33.75" customHeight="1">
+    </row>
+    <row r="19" spans="1:11" ht="33.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -1332,9 +1329,8 @@
         <v>67</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" ht="48" customHeight="1">
+    </row>
+    <row r="20" spans="1:11" ht="48" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1364,9 +1360,8 @@
         <v>68</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" ht="18.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:11" ht="18.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1396,14 +1391,10 @@
         <v>71</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J16" r:id="rId1" display="status=200||lastName=nottiedtosubscription||email=test.user101@clarivate.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed script in drassologin test data
</commit_message>
<xml_diff>
--- a/src/test/test-data/SsoLoginTestData.xlsx
+++ b/src/test/test-data/SsoLoginTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -306,9 +306,6 @@
   <si>
     <t>{"RelayState":"(OPQA-5697_relayState)",
 "SAMLResponse":"InvalidSAML"}</t>
-  </si>
-  <si>
-    <t>status=200||lastName=nottiedtosubscription||email=test.user101@clarivate.com</t>
   </si>
 </sst>
 </file>
@@ -739,10 +736,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <pane ySplit="900" topLeftCell="A10" activePane="bottomLeft"/>
       <selection activeCell="H5" sqref="H5"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L21"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1233,7 +1230,7 @@
         <v>40</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="K16" s="2"/>
     </row>

</xml_diff>

<commit_message>
fixed failed scripts in SSO login module
</commit_message>
<xml_diff>
--- a/src/test/test-data/SsoLoginTestData.xlsx
+++ b/src/test/test-data/SsoLoginTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
   <si>
     <t>TESTNAME</t>
   </si>
@@ -87,9 +92,6 @@
     <t>?clientId=ass0bfb-0126-4186-b27e-b5cc4619e7a3&amp;app=neon&amp;appurl=https://access.dev-stable.clarivate.com</t>
   </si>
   <si>
-    <t>?clientId=525d0bfb-0126-4186-b27e-b5cc4619e7a3&amp;app=dra&amp;appurl=https://access.dev-stable.clarivate.com</t>
-  </si>
-  <si>
     <t>1POAUTH</t>
   </si>
   <si>
@@ -294,25 +296,31 @@
     <t>content-type=application/x-www-form-urlencoded</t>
   </si>
   <si>
-    <t>{"RelayState":"(OPQA-5697_relayState)",
+    <t>/sso/saml2/authorize</t>
+  </si>
+  <si>
+    <t>?clientId=525d0bfb-0126-4186-b27e-b5cc4619e7a3&amp;app=ddra&amp;appurl=https://www.invalid.com</t>
+  </si>
+  <si>
+    <t>?clientId=RAdneiT8SMGtuEnljBFWGA&amp;app=dra&amp;appurl=https://access.dev-stable.clarivate.com</t>
+  </si>
+  <si>
+    <t>authenticationResponse.relayState</t>
+  </si>
+  <si>
+    <t>{"RelayState":"(OPQA-5697_authenticationResponse.relayState)",
 "SAMLResponse":"PHNhbWxwOlJlc3BvbnNlIHhtbG5zOnNhbWxwPSJ1cm46b2FzaXM6bmFtZXM6dGM6U0FNTDoyLjA6cHJvdG9jb2wiIHhtbG5zOnNhbWw9InVybjpvYXNpczpuYW1lczp0YzpTQU1MOjIuMDphc3NlcnRpb24iIERlc3RpbmF0aW9uPSJodHRwOi8vYWNjZXNzLmRldi1zdGFibGUuY2xhcml2YXRlLmNvbS9hcGkvc3NvL3NhbWwyL2F1dGhvcml6ZSIgSUQ9IklEXzRjZmI5M2IxLTE4ZGUtNDE1OS1iYjY2LTMwNzMwYjg3YjVhZCIgSW5SZXNwb25zZVRvPSJfLTU5OTk1MDc1NjQ1NzE3NjYwMTYiIElzc3VlSW5zdGFudD0iMjAxOC0wMi0yN1QyMjozOToyMy4yOTJaIiBWZXJzaW9uPSIyLjAiPjxzYW1sOklzc3Vlcj5odHRwOi8vZWMyLTUyLTMzLTEzLTczLnVzLXdlc3QtMi5jb21wdXRlLmFtYXpvbmF3cy5jb206ODA4MC9hdXRoL3JlYWxtcy9QbGF0Zm9ybS1JQU08L3NhbWw6SXNzdWVyPjxzYW1scDpTdGF0dXM+PHNhbWxwOlN0YXR1c0NvZGUgVmFsdWU9InVybjpvYXNpczpuYW1lczp0YzpTQU1MOjIuMDpzdGF0dXM6U3VjY2VzcyIvPjwvc2FtbHA6U3RhdHVzPjxzYW1sOkFzc2VydGlvbiB4bWxucz0idXJuOm9hc2lzOm5hbWVzOnRjOlNBTUw6Mi4wOmFzc2VydGlvbiIgSUQ9IklEXzQzZGM5YWViLWY4M2UtNDBiNS1hYjcwLWYyYWEyMDRjOThhYiIgSXNzdWVJbnN0YW50PSIyMDE4LTAyLTI3VDIyOjM5OjIzLjI5MVoiIFZlcnNpb249IjIuMCI+PHNhbWw6SXNzdWVyPmh0dHA6Ly9lYzItNTItMzMtMTMtNzMudXMtd2VzdC0yLmNvbXB1dGUuYW1hem9uYXdzLmNvbTo4MDgwL2F1dGgvcmVhbG1zL1BsYXRmb3JtLUlBTTwvc2FtbDpJc3N1ZXI+PHNhbWw6U3ViamVjdD48c2FtbDpOYW1lSUQgRm9ybWF0PSJ1cm46b2FzaXM6bmFtZXM6dGM6U0FNTDoyLjA6bmFtZWlkLWZvcm1hdDp0cmFuc2llbnQiPkctMTlmYzdjNjgtZGIxNS00YzllLWJhODAtMzgwZWNhN2U4MDZjPC9zYW1sOk5hbWVJRD48c2FtbDpTdWJqZWN0Q29uZmlybWF0aW9uIE1ldGhvZD0idXJuOm9hc2lzOm5hbWVzOnRjOlNBTUw6Mi4wOmNtOmJlYXJlciI+PHNhbWw6U3ViamVjdENvbmZpcm1hdGlvbkRhdGEgSW5SZXNwb25zZVRvPSJfLTU5OTk1MDc1NjQ1NzE3NjYwMTYiIE5vdE9uT3JBZnRlcj0iMjAxOC0wMi0yN1QyMjo0NDoyMS4yOTFaIiBSZWNpcGllbnQ9Imh0dHA6Ly9hY2Nlc3MuZGV2LXN0YWJsZS5jbGFyaXZhdGUuY29tL2FwaS9zc28vc2FtbDIvYXV0aG9yaXplIi8+PC9zYW1sOlN1YmplY3RDb25maXJtYXRpb24+PC9zYW1sOlN1YmplY3Q+PHNhbWw6Q29uZGl0aW9ucyBOb3RCZWZvcmU9IjIwMTgtMDItMjdUMjI6Mzk6MjEuMjkxWiIgTm90T25PckFmdGVyPSIyMDE4LTAyLTI3VDIyOjQwOjIxLjI5MVoiPjxzYW1sOkF1ZGllbmNlUmVzdHJpY3Rpb24+PHNhbWw6QXVkaWVuY2U+dXJuOm1hY2U6ZmVkZXJhdGlvbi5vcmcuYXU6dGVzdGZlZDpzaGliMjwvc2FtbDpBdWRpZW5jZT48L3NhbWw6QXVkaWVuY2VSZXN0cmljdGlvbj48L3NhbWw6Q29uZGl0aW9ucz48c2FtbDpBdHRyaWJ1dGVTdGF0ZW1lbnQ+PHNhbWw6QXR0cmlidXRlIE5hbWU9ImFwcGxpY2F0aW9uIiBOYW1lRm9ybWF0PSJ1cm46b2FzaXM6bmFtZXM6dGM6U0FNTDoyLjA6YXR0cm5hbWUtZm9ybWF0OmJhc2ljIj48c2FtbDpBdHRyaWJ1dGVWYWx1ZSB4bWxuczp4cz0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEiIHhtbG5zOnhzaT0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEtaW5zdGFuY2UiIHhzaTp0eXBlPSJ4czpzdHJpbmciPkRSQTwvc2FtbDpBdHRyaWJ1dGVWYWx1ZT48L3NhbWw6QXR0cmlidXRlPjxzYW1sOkF0dHJpYnV0ZSBOYW1lPSJmaXJzdE5hbWUiIE5hbWVGb3JtYXQ9InVybjpvYXNpczpuYW1lczp0YzpTQU1MOjIuMDphdHRybmFtZS1mb3JtYXQ6YmFzaWMiPjxzYW1sOkF0dHJpYnV0ZVZhbHVlIHhtbG5zOnhzPSJodHRwOi8vd3d3LnczLm9yZy8yMDAxL1hNTFNjaGVtYSIgeG1sbnM6eHNpPSJodHRwOi8vd3d3LnczLm9yZy8yMDAxL1hNTFNjaGVtYS1pbnN0YW5jZSIgeHNpOnR5cGU9InhzOnN0cmluZyI+dGVzdC51c2VyPC9zYW1sOkF0dHJpYnV0ZVZhbHVlPjwvc2FtbDpBdHRyaWJ1dGU+PHNhbWw6QXR0cmlidXRlIE5hbWU9Imxhc3ROYW1lIiBOYW1lRm9ybWF0PSJ1cm46b2FzaXM6bmFtZXM6dGM6U0FNTDoyLjA6YXR0cm5hbWUtZm9ybWF0OmJhc2ljIj48c2FtbDpBdHRyaWJ1dGVWYWx1ZSB4bWxuczp4cz0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEiIHhtbG5zOnhzaT0iaHR0cDovL3d3dy53My5vcmcvMjAwMS9YTUxTY2hlbWEtaW5zdGFuY2UiIHhzaTp0eXBlPSJ4czpzdHJpbmciPm1pc3NpbmcuZW1haWw8L3NhbWw6QXR0cmlidXRlVmFsdWU+PC9zYW1sOkF0dHJpYnV0ZT48L3NhbWw6QXR0cmlidXRlU3RhdGVtZW50Pjwvc2FtbDpBc3NlcnRpb24+PC9zYW1scDpSZXNwb25zZT4="}</t>
   </si>
   <si>
-    <t>/sso/saml2/authorize</t>
-  </si>
-  <si>
-    <t>?clientId=525d0bfb-0126-4186-b27e-b5cc4619e7a3&amp;app=ddra&amp;appurl=https://www.invalid.com</t>
-  </si>
-  <si>
-    <t>{"RelayState":"(OPQA-5697_relayState)",
+    <t>{"RelayState":"(OPQA-5697_authenticationResponse.relayState)",
 "SAMLResponse":"InvalidSAML"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,7 +500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -524,9 +532,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,6 +567,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -733,16 +743,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A10" activePane="bottomLeft"/>
-      <selection activeCell="H5" sqref="H5"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1" collapsed="1"/>
@@ -756,7 +764,7 @@
     <col min="11" max="11" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,12 +802,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -821,12 +829,12 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -848,12 +856,12 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -866,23 +874,23 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30">
+      <c r="K4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -900,16 +908,16 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -922,37 +930,37 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="30.75" customHeight="1">
+    <row r="7" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="7" t="s">
@@ -962,430 +970,430 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="23.25" customHeight="1">
+    <row r="8" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="75">
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="29.25" customHeight="1">
+    <row r="10" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="29.25" customHeight="1">
+    <row r="11" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="29.25" customHeight="1">
+    <row r="12" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="29.25" customHeight="1">
+    <row r="13" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" ht="29.25" customHeight="1">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="32.25" customHeight="1">
+    <row r="15" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="43.5" customHeight="1">
+    <row r="16" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>15</v>
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="44.25" customHeight="1">
+    <row r="17" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="48.75" customHeight="1">
+    <row r="18" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="33.75" customHeight="1">
+    <row r="19" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="48" customHeight="1">
+    <row r="20" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K21" s="2"/>
     </row>
@@ -1396,24 +1404,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>